<commit_message>
some trash from server
</commit_message>
<xml_diff>
--- a/files/1-курс-бакалавриат-ОФО-48.xlsx
+++ b/files/1-курс-бакалавриат-ОФО-48.xlsx
@@ -15,10 +15,70 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ИУПСиБК 1 курс" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="Z_267C3CE3_12D1_42A7_AE8A_91549D6C5A72_.wvu.PrintArea" localSheetId="0" hidden="1">'ИГУиП 1 курс'!$A$1:$M$57</definedName>
+    <definedName name="Z_275EF655_CA8F_4C06_9BBE_6528C8591DF3_.wvu.PrintArea" localSheetId="0" hidden="1">'ИГУиП 1 курс'!$A$1:$M$56</definedName>
+    <definedName name="Z_34939890_54CB_44B5_AA6A_F4AE45B6E4B5_.wvu.PrintArea" localSheetId="0" hidden="1">'ИГУиП 1 курс'!$A$1:$M$56</definedName>
+    <definedName name="Z_82FF29C3_C992_47D7_B1E4_D6954C709F01_.wvu.PrintArea" localSheetId="0" hidden="1">'ИГУиП 1 курс'!$A$1:$M$56</definedName>
+    <definedName name="Z_99487DB8_288A_44E1_8591_9E25D3654283_.wvu.PrintArea" localSheetId="0" hidden="1">'ИГУиП 1 курс'!$A$1:$M$59</definedName>
+    <definedName name="Z_9CF115AF_64D0_44DE_8848_18CE4B1A7306_.wvu.PrintArea" localSheetId="0" hidden="1">'ИГУиП 1 курс'!$A$1:$M$56</definedName>
+    <definedName name="Z_A45D948D_1882_47E4_B420_D1562C5BEF3B_.wvu.PrintArea" localSheetId="0" hidden="1">'ИГУиП 1 курс'!$A$1:$M$61</definedName>
+    <definedName name="Z_A7A98B23_589F_47AA_865D_272CDEBCD96B_.wvu.PrintArea" localSheetId="0" hidden="1">'ИГУиП 1 курс'!$A$1:$M$56</definedName>
+    <definedName name="Z_B3C82B95_44DA_4B4A_9C56_F713C3B229B7_.wvu.PrintArea" localSheetId="0" hidden="1">'ИГУиП 1 курс'!$C$1:$M$61</definedName>
+    <definedName name="Z_B7C456BE_EF59_4A2E_8C4E_1F8FE493FCB9_.wvu.PrintArea" localSheetId="0" hidden="1">'ИГУиП 1 курс'!$A$1:$M$56</definedName>
+    <definedName name="Z_D7398314_CF85_44B7_AC43_71E5DC206045_.wvu.PrintArea" localSheetId="0" hidden="1">'ИГУиП 1 курс'!$A$1:$M$61</definedName>
+    <definedName name="Z_E6ED7FAC_B2D1_47FB_BE0A_759CE492F51C_.wvu.PrintArea" localSheetId="0" hidden="1">'ИГУиП 1 курс'!$A$1:$M$56</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'ИГУиП 1 курс'!$A$1:$M$56</definedName>
+    <definedName name="Z_267C3CE3_12D1_42A7_AE8A_91549D6C5A72_.wvu.PrintArea" localSheetId="1" hidden="1">'ИМ 1 курс'!$A$1:$N$56</definedName>
+    <definedName name="Z_275EF655_CA8F_4C06_9BBE_6528C8591DF3_.wvu.PrintArea" localSheetId="1" hidden="1">'ИМ 1 курс'!$A$1:$N$56</definedName>
+    <definedName name="Z_34939890_54CB_44B5_AA6A_F4AE45B6E4B5_.wvu.PrintArea" localSheetId="1" hidden="1">'ИМ 1 курс'!$A$1:$N$56</definedName>
+    <definedName name="Z_82FF29C3_C992_47D7_B1E4_D6954C709F01_.wvu.PrintArea" localSheetId="1" hidden="1">'ИМ 1 курс'!$J$19:$N$24</definedName>
+    <definedName name="Z_99487DB8_288A_44E1_8591_9E25D3654283_.wvu.PrintArea" localSheetId="1" hidden="1">'ИМ 1 курс'!$A$1:$N$62</definedName>
+    <definedName name="Z_9CF115AF_64D0_44DE_8848_18CE4B1A7306_.wvu.PrintArea" localSheetId="1" hidden="1">'ИМ 1 курс'!$J$19:$N$24</definedName>
+    <definedName name="Z_A45D948D_1882_47E4_B420_D1562C5BEF3B_.wvu.PrintArea" localSheetId="1" hidden="1">'ИМ 1 курс'!$A$1:$N$56</definedName>
+    <definedName name="Z_A7A98B23_589F_47AA_865D_272CDEBCD96B_.wvu.PrintArea" localSheetId="1" hidden="1">'ИМ 1 курс'!$B$6:$F$56</definedName>
+    <definedName name="Z_B3C82B95_44DA_4B4A_9C56_F713C3B229B7_.wvu.PrintArea" localSheetId="1" hidden="1">'ИМ 1 курс'!$B$1:$N$62</definedName>
+    <definedName name="Z_B7C456BE_EF59_4A2E_8C4E_1F8FE493FCB9_.wvu.PrintArea" localSheetId="1" hidden="1">'ИМ 1 курс'!$J$19:$N$24</definedName>
+    <definedName name="Z_D7398314_CF85_44B7_AC43_71E5DC206045_.wvu.PrintArea" localSheetId="1" hidden="1">'ИМ 1 курс'!$A$1:$N$56</definedName>
+    <definedName name="Z_E6ED7FAC_B2D1_47FB_BE0A_759CE492F51C_.wvu.PrintArea" localSheetId="1" hidden="1">'ИМ 1 курс'!$A$1:$N$56</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'ИМ 1 курс'!$J$19:$N$24</definedName>
+    <definedName name="Z_267C3CE3_12D1_42A7_AE8A_91549D6C5A72_.wvu.PrintArea" localSheetId="2" hidden="1">'ИУПСиБК, ИИС 1 курс'!$A$1:$M$56</definedName>
+    <definedName name="Z_275EF655_CA8F_4C06_9BBE_6528C8591DF3_.wvu.PrintArea" localSheetId="2" hidden="1">'ИУПСиБК, ИИС 1 курс'!$A$1:$M$56</definedName>
+    <definedName name="Z_34939890_54CB_44B5_AA6A_F4AE45B6E4B5_.wvu.PrintArea" localSheetId="2" hidden="1">'ИУПСиБК, ИИС 1 курс'!$A$1:$M$56</definedName>
+    <definedName name="Z_82FF29C3_C992_47D7_B1E4_D6954C709F01_.wvu.PrintArea" localSheetId="2" hidden="1">'ИУПСиБК, ИИС 1 курс'!$A$1:$M$56</definedName>
+    <definedName name="Z_99487DB8_288A_44E1_8591_9E25D3654283_.wvu.PrintArea" localSheetId="2" hidden="1">'ИУПСиБК, ИИС 1 курс'!$A$1:$M$56</definedName>
+    <definedName name="Z_9CF115AF_64D0_44DE_8848_18CE4B1A7306_.wvu.PrintArea" localSheetId="2" hidden="1">'ИУПСиБК, ИИС 1 курс'!$A$1:$M$56</definedName>
+    <definedName name="Z_A45D948D_1882_47E4_B420_D1562C5BEF3B_.wvu.PrintArea" localSheetId="2" hidden="1">'ИУПСиБК, ИИС 1 курс'!$A$1:$M$56</definedName>
+    <definedName name="Z_A7A98B23_589F_47AA_865D_272CDEBCD96B_.wvu.PrintArea" localSheetId="2" hidden="1">'ИУПСиБК, ИИС 1 курс'!$A$1:$M$56</definedName>
+    <definedName name="Z_B3C82B95_44DA_4B4A_9C56_F713C3B229B7_.wvu.PrintArea" localSheetId="2" hidden="1">'ИУПСиБК, ИИС 1 курс'!$A$1:$M$56</definedName>
+    <definedName name="Z_B7C456BE_EF59_4A2E_8C4E_1F8FE493FCB9_.wvu.PrintArea" localSheetId="2" hidden="1">'ИУПСиБК, ИИС 1 курс'!$A$1:$M$56</definedName>
+    <definedName name="Z_D7398314_CF85_44B7_AC43_71E5DC206045_.wvu.PrintArea" localSheetId="2" hidden="1">'ИУПСиБК, ИИС 1 курс'!$A$1:$M$56</definedName>
+    <definedName name="Z_E6ED7FAC_B2D1_47FB_BE0A_759CE492F51C_.wvu.PrintArea" localSheetId="2" hidden="1">'ИУПСиБК, ИИС 1 курс'!$A$1:$M$56</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'ИИС 1 курс'!$A$1:$M$56</definedName>
+    <definedName name="Z_267C3CE3_12D1_42A7_AE8A_91549D6C5A72_.wvu.PrintArea" localSheetId="3" hidden="1">'ИЭиФ 1 курс'!$B$1:$O$56</definedName>
+    <definedName name="Z_275EF655_CA8F_4C06_9BBE_6528C8591DF3_.wvu.PrintArea" localSheetId="3" hidden="1">'ИЭиФ 1 курс'!$B$1:$O$56</definedName>
+    <definedName name="Z_34939890_54CB_44B5_AA6A_F4AE45B6E4B5_.wvu.PrintArea" localSheetId="3" hidden="1">'ИЭиФ 1 курс'!$B$1:$O$56</definedName>
+    <definedName name="Z_82FF29C3_C992_47D7_B1E4_D6954C709F01_.wvu.PrintArea" localSheetId="3" hidden="1">'ИЭиФ 1 курс'!$B$1:$O$56</definedName>
+    <definedName name="Z_99487DB8_288A_44E1_8591_9E25D3654283_.wvu.PrintArea" localSheetId="3" hidden="1">'ИЭиФ 1 курс'!$B$1:$O$56</definedName>
+    <definedName name="Z_9CF115AF_64D0_44DE_8848_18CE4B1A7306_.wvu.PrintArea" localSheetId="3" hidden="1">'ИЭиФ 1 курс'!$B$1:$O$56</definedName>
+    <definedName name="Z_A45D948D_1882_47E4_B420_D1562C5BEF3B_.wvu.PrintArea" localSheetId="3" hidden="1">'ИЭиФ 1 курс'!$B$1:$O$56</definedName>
+    <definedName name="Z_A7A98B23_589F_47AA_865D_272CDEBCD96B_.wvu.PrintArea" localSheetId="3" hidden="1">'ИЭиФ 1 курс'!$B$1:$O$56</definedName>
+    <definedName name="Z_B3C82B95_44DA_4B4A_9C56_F713C3B229B7_.wvu.PrintArea" localSheetId="3" hidden="1">'ИЭиФ 1 курс'!$B$1:$O$56</definedName>
+    <definedName name="Z_B7C456BE_EF59_4A2E_8C4E_1F8FE493FCB9_.wvu.PrintArea" localSheetId="3" hidden="1">'ИЭиФ 1 курс'!$B$1:$O$56</definedName>
+    <definedName name="Z_D7398314_CF85_44B7_AC43_71E5DC206045_.wvu.PrintArea" localSheetId="3" hidden="1">'ИЭиФ 1 курс'!$B$1:$O$56</definedName>
+    <definedName name="Z_E6ED7FAC_B2D1_47FB_BE0A_759CE492F51C_.wvu.PrintArea" localSheetId="3" hidden="1">'ИЭиФ 1 курс'!$B$1:$O$56</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'ИЭиФ 1 курс'!$B$1:$O$56</definedName>
+    <definedName name="Z_267C3CE3_12D1_42A7_AE8A_91549D6C5A72_.wvu.PrintArea" localSheetId="5" hidden="1">'3 курс'!$A$1:$Q$68</definedName>
+    <definedName name="Z_275EF655_CA8F_4C06_9BBE_6528C8591DF3_.wvu.PrintArea" localSheetId="5" hidden="1">'3 курс'!$A$1:$Q$68</definedName>
+    <definedName name="Z_34939890_54CB_44B5_AA6A_F4AE45B6E4B5_.wvu.PrintArea" localSheetId="5" hidden="1">'3 курс'!$A$1:$Q$68</definedName>
+    <definedName name="Z_82FF29C3_C992_47D7_B1E4_D6954C709F01_.wvu.PrintArea" localSheetId="5" hidden="1">'3 курс'!$A$1:$Q$68</definedName>
+    <definedName name="Z_99487DB8_288A_44E1_8591_9E25D3654283_.wvu.PrintArea" localSheetId="5" hidden="1">'3 курс'!$A$1:$Q$68</definedName>
+    <definedName name="Z_9CF115AF_64D0_44DE_8848_18CE4B1A7306_.wvu.PrintArea" localSheetId="5" hidden="1">'3 курс'!$A$1:$Q$68</definedName>
+    <definedName name="Z_A45D948D_1882_47E4_B420_D1562C5BEF3B_.wvu.PrintArea" localSheetId="5" hidden="1">'3 курс'!$A$1:$Q$68</definedName>
+    <definedName name="Z_A7A98B23_589F_47AA_865D_272CDEBCD96B_.wvu.PrintArea" localSheetId="5" hidden="1">'3 курс'!$A$1:$Q$68</definedName>
+    <definedName name="Z_B3C82B95_44DA_4B4A_9C56_F713C3B229B7_.wvu.PrintArea" localSheetId="5" hidden="1">'3 курс'!$A$1:$Q$68</definedName>
+    <definedName name="Z_B7C456BE_EF59_4A2E_8C4E_1F8FE493FCB9_.wvu.PrintArea" localSheetId="5" hidden="1">'3 курс'!$A$1:$Q$68</definedName>
+    <definedName name="Z_D7398314_CF85_44B7_AC43_71E5DC206045_.wvu.PrintArea" localSheetId="5" hidden="1">'3 курс'!$A$1:$Q$68</definedName>
+    <definedName name="Z_E6ED7FAC_B2D1_47FB_BE0A_759CE492F51C_.wvu.PrintArea" localSheetId="5" hidden="1">'3 курс'!$A$1:$Q$68</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'3 курс'!$A$1:$Q$68</definedName>
   </definedNames>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>

</xml_diff>